<commit_message>
Get daily reddit data: Tue Feb 13 08:08:56 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_18.xlsx
+++ b/data/2024_02_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C479"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3032 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1apobzp</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Google can't seem to comprehend this question, so I've got to come to fellow humans for consult. Question in post, PLEASE HELP IF YOU CAN 🙏🏼</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apobzp/google_cant_seem_to_comprehend_this_question_so/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1apo7fu</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>These took 6 days 😭</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qofuko76bic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1apo2wh</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>I want to take off acrylics and just keep the length on my natural nails. Suggestions?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3eetoyj4bic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1apnw76</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Holo/abstract nails I did</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjbl2x772bic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1apnmxp</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dtd7lw1zaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1apnhvd</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Which nail shape suits my hands better, square or oval?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apnhvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1apm38g</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Obsessed 🤩</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbfcmxebiaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1aplzuy</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Jelly ombré</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gp6ji5dhaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1aplq7d</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>my favorite spring nails</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/884dch4peaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1aplf59</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Good or bad?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61ucpcbpbaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1apleun</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Did my nails for Superbowl! Chiefs Kingdom! ❤️💛🤍</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apleun</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1apkya5</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Best LED lamp?</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbq66ngd7aic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1apkobm</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>I butchered my nails by trying to learn gel at home.</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apkobm</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1apjdb6</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>new nails!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf7rvz41t9ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1apjc3c</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>fill in question</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apjc3c/fill_in_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1apj1d5</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Why won’t anything stay on my nails?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ie42157q9ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1apiirx</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Happy Valentines Nails 💌</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmvisrwsl9ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1api9fv</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Acrylic powder 3 months progress</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1api9fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1aphy2g</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>I love my new nails!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s54hlrdrg9ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1aphs2n</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>strawberry teddies🧸🍓</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bllhf0ohf9ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1aphp56</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aphp56</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1aphd12</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Anxiety...defeated for now</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nj7qmhwb9ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1aph5c9</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Help with gel polish!</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aph5c9/help_with_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1apglnf</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>New mani - feeling pretty</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1o88y8h59ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1apgkzk</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Which chrome powders does Padena use?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apgkzk/which_chrome_powders_does_padena_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1apgel4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Spikes?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4j7d5iu39ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1apga12</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>My first time using press on nails :)</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apga12</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1apg4w0</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>These gel nails a whole 48 hours...</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d57ksslm19ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1apg0tg</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>First time doing a long coffin set</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1amfw7p09ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1apfyf1</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>My simple Valentine’s Day nails 💋</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apfyf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1apfx46</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Acylic Beginner</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42zo9ifvz8ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1apfno6</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>New set, wanted something different.🤗</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxkj0hiox8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1apfbc4</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My friend asked me to do her birthday nails</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b24hyfywu8ic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1apeuaz</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>quick ombre set❤️</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7l7xh67r8ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1apepx7</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>How to remove stains from orange?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apepx7/how_to_remove_stains_from_orange/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1apelle</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Sea glass nails I did on myself, one week later</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kk3linibp8ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1apek9u</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>I got new nails today, I’m in love 🥰</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30zjq141p8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1apefuz</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Wrinkly hands</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pm732ur3o8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1apedjx</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Love my nail tech!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apedjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1apecqk</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apecqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1apdv4a</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>valentines nails!</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkpxmhbqj8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1apdk62</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>In love with my grungy Valentine's nails 💜🙌</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apdk62</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1apd8qz</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>I always avoided pastel colors…</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/233ra9v1f8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1apd5wi</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Basic nails for Valentine's Day! Hope you receive lots of love!</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqz29obge8ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1apb8xq</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>My new set 😭✨🖤</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apb8xq</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1apawfv</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Chinese New Year inspired nails ʚ(* ´꒳` *)ɞ🐉🧧💗</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apawfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1apbit0</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Valentine’s nails🫶🏻💌</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0likv08j28ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1apbg17</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Press-on nails are my new go to</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cebjkkpy18ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1apb51t</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>I live for an emerald green moment</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sdapmfrz7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1apb458</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Really mesmerizing colors😍</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwrkt8vkz7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ap74en</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Beginner Level Advice/Stuggling to Do Nails</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ap74en/beginner_level_advicestuggling_to_do_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1apajr5</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>What color nails should I wear with this dress?</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt23swjlv7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1apah2b</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Press On Hack</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apah2b/press_on_hack/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1apaey6</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>cute valentine's nails ‹𝟹</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apaey6</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1apabrw</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Press-ons: Super glue?</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apabrw/pressons_super_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ap9z0b</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>How long did it take for you to master gelx. Still takes me about an hour a hand. What about dip, is it easier? Just now learning all things diy nails, feeling overwhelmed.</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap9z0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ap9so4</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>valentines holo mani of my dreams 🤩</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap9so4</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ap9d9a</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Tried gel tips for the first time.</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6z3omdzdn7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ap8v6d</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>my natural nails. 🥀</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgcahqaxj7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ap8cnb</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Xoxo</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9zbq2gag7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ap89zw</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>My Valentine nails</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hdx0pm3tf7ic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ap89fv</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>What do we think about this color palette?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap89fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ap867r</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>gel x valentine’s day nails</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcqg82f1f7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ap85s1</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Valentines day nails</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58we9lpxe7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ap811v</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>valentines day set 🥰</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kpnb7vzd7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ap801n</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>New set by me! Not sure what to call it tho!</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap801n</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ap7wtp</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Todays client.</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ae2nvc5d7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ap7jwm</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Happy accidents😅</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap7jwm</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ap7jqw</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Leftover gel.. is this normal?</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkuzqhuja7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ap7e26</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Anti-Valentine Day Nails.</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/41l1c3df97ic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1ap7a8j</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Some more pics of my nails 😍</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap7a8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ap72q7</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jletbqe877ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ap718w</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>phases of the moon nails</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap718w</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ap62pq</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>New claws 🖤</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap62pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ap5saw</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>What would you recommend for longevity and nail health?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ap5saw/what_would_you_recommend_for_longevity_and_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ap5n95</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>My first acrylic nails ✨</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gopwdjv1x6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ap5fsb</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Nails are too strong</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap5fsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ap5i42</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Got my nails done at a new salon!</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap5i42</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ap5fxq</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>(Beginner) Orange and Blue nails!</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap5fxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ap5d5s</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>DIY Vday Set ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t069mk32v6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ap5alv</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Plaid</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nn7d1xiku6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ap49tr</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>classic</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap49tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ap3nvm</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>coquette inspired nails!</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap3nvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ap3kqj</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I suck at nail art, but love my nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap3kqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ap3kla</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>What are your favorite gel nail polish brands?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ap3kla/what_are_your_favorite_gel_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ap3ivb</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Should I clip them all?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap3ivb</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ap3gwx</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Queen of hearts</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap3gwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ap3frq</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Boondocks nails! Def one of my fav sets</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2niwp98ah6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ap3aon</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap3aon</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ap33ri</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b972y4qre6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ap2tjm</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Anyone know what this is?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap2tjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ap22w8</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Painted some chrome hearts</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9bvoliq66ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1ap1pwr</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>A Valentine's Day inspired set that I did on myself. 💅🏿💘</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap1pwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1ap1gzb</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Just finished these!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ta2aprls16ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1ap00wq</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Trying to grow out my nails… what do I do when this happens?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klb0uzx7p5ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1ap21m2</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>I told her I wanted yeehaw neon valentines, I think she smashed it</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l87mey2g66ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ap1nyq</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Pink neon hearts for Valentines 💕</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap1nyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ap1gg9</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>A husband on a mission - 25th wedding anniversary nails are now gone, but she didn't really want Valentine's nails.</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap1gg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ap1fst</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Simple and sweet</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okjcn8ai16ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ap0u5i</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>I got the job! These are my celebratory nails</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q87qha3iw5ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1apn5vp</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Swamp Sparrow in Love</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apn5vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1apm7fu</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Too many releases (aka Old Woman Yells at Cloud).</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apm7fu/too_many_releases_aka_old_woman_yells_at_cloud/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1aplr7f</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>My baby's first mani</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0iypdlgzeaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1aplqlx</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Looking for lacquer suggestions like this snowy look</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4bs488teaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1aplc23</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Planning First Cirque Order</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aplc23</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1apl689</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Did my nails to support my Superbowl team! Chiefs Kingdom! 🤍💛❤️</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apl689</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1apkwey</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Zenon-inspired pink skittle</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apkwey</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1apjcrs</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>The perfect combo</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apjcrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1apivzi</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Coolest polish I've owned</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apivzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1aph4ix</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>There’s no place like…</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aph4ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1aph3qs</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>💜✨️</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aph3qs</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1apghzd</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>ILNP Cameo (h) is the perfect barely-festive color for my fellow Valentine’s Day skeptics!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z8mpcvm49ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1apghkw</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>opi gel polish #92 / gel x stiletto tips shaped to almond</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apghkw</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1apghad</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Valentine's nails ❤️🩷</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apghad</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1apg5ax</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Decided to try a more natural look this time</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pc9qt0q19ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1apg1xr</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>What the hell am I supposed to do with my sidewalls</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apg1xr/what_the_hell_am_i_supposed_to_do_with_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1apfv32</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>“Palate cleanser” colors are my go-to colors</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apfv32</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1apfswa</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Haku ✨️</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apfswa</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1apfc6l</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Pearls on Mars</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5591i14v8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1apekke</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Looking for a pink rose gold</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mpa00h3p8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1apejgd</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Mother/Son manis!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apejgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1apegk9</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Top coats that are cruelty free and vegan</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apegk9/top_coats_that_are_cruelty_free_and_vegan/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1apdt6j</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Fancy Gloss “Glowing Mushroom”</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apdt6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1apdol1</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Negative space mani</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p0p5bjdi8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1apd9jw</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Zoya Blaze for Valentines 💝</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5fty7d8f8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1apcgyn</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Found the ultimate Valentines color</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apcgyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1apbvs7</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>My nails are constantly peeling/ breaking. Should I use a ridge filler base before painting?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apbvs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1apbhao</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Brand new bottle of Essie Smooth-E base is… runny and yellow (???)</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9uxc7wd828ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ap7e5b</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Mooncat Spaceoddity</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u87cs21g97ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1apaxhi</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>EDM Written Invitation vs. Cirque Déjà Vu</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apaxhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1apag83</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>What nail shape best fits my hand/finger shape?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apag83/what_nail_shape_best_fits_my_handfinger_shape/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1apaex2</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Anyone know how to get rid of white flecks from matte tc?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apaex2</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1apa6uo</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>The ✨aesthetic✨</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p06vq9n1t7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1apa6fv</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>First (and last?) Valentine's Day set of 2024</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jw5apz00t7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ap9fda</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Mani</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ncj2ourn7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ap7hik</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Another set of groundbreaking vday nails</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imgnfi74a7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ap6a93</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Poparazzi - Dancing In The Meadow</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap6a93</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ap68lt</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>I bought my first 5 ILNP polishes in August…</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxrxyhid17ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ap5v7s</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Ethereal Sixth Station</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap5v7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ap5pg4</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Back on my nail bullshit after a category 5 heartbreak 💔</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap5pg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ap59jq</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>foils on regular polish</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap59jq</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ap5l5n</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Is there a way to clean topcoat brushes?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5ecg4bnw6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ap5i6z</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Lyn B Designs</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ap5i6z/lyn_b_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ap5hrv</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Probably my last Valentine's nails...</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap5hrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ap5b4v</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Experiments with Crackle Nail Polish</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la6tdc6ou6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ap4l5r</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Nail peeling more due to strengthener. Any other options?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ap4l5r/nail_peeling_more_due_to_strengthener_any_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ap4jz2</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Morning Glory</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qoq1j7tcp6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ap4ixm</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Tips (pun intended) to make regular nail polish last longer on natural nails?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ap4ixm/tips_pun_intended_to_make_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ap3y9s</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Valentines day ♡</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap3y9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ap3lnk</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>My Valentine's Day polish :)</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vsvkvtkei6ic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ap2uud</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Valentine's Nails</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0kyiaxlvc6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ap2twq</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Year of the Dragon Mani</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbihiuyoc6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ap2iux</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>and the boolba saga continues!</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap2iux</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1ap2b5c</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>First time trying ORLY... omg! I'm in love (Beautifully Bizarre)</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap2b5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1ap29rx</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>⭐️ Heavenmetal ⭐️</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap29rx</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1ap20aw</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Mooncat's Merkitten</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekbfivv466ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1ap1jz6</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>For Valentine’s 🌷💜</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjmszrgg26ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1ap1ca3</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Valentine's mani 🤍❤️</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y2mmfgp06ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1ap17bz</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Valentine's nails, part 2</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0nimfvjz5ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1ap0qkx</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Jen &amp; Berries - Raspberry Parade</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zuqjl46lv5ic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ap0lki</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Favorite blurring bases? (Pic of Valentine’s Day mani and kitten for attention.)</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d66axsvgu5ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ap0h5d</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Help, removed nail polish and nails are damaged, what should I do?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap0h5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ap011a</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>LynB strikes again</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4ejc6pbp5ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1aoxhe9</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aoxhe9/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1apnbzi</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Some press ons I made</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaaicgljvaic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1apd596</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Nail Art Tutorials</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://youtube.com/watch?v=Wi4AcKZpKsg&amp;si=vjpH-MUcZ0S2BUJB</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1apkd5d</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Hand painted and sculpted press-on nails</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u0gv6wvj1aic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1apjcg4</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>I did for myself…</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkbwoj3us9ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1apibda</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Acrylic powder 3 months progress</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apibda</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1apgjrs</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>What chrome powders does Padena use?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1apgjrs/what_chrome_powders_does_padena_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1apexiq</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>IG Collab Nail Art</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apexiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1apepd5</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Pink Polka Dots</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zgnp9tz4q8ic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1apdheh</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Winter meets spring</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hh60r3gug8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1apd802</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>My 1 Year Nailaversery!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v64bwt5we8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1apb1jt</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>In love with these</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgofazo2z7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1apae71</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>cute valentine's day nails ‹𝟹</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apae71</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1ap3v2e</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>By: NailzXshanti</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ap3v2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1ap3b2e</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day nails!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvtw3qybg6ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Feb 14 08:08:13 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_18.xlsx
+++ b/data/2024_02_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C479"/>
+  <dimension ref="A1:C661"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8576,6 +8576,3100 @@
         </is>
       </c>
     </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1aqhr7y</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Some of my recent nail art on all natural nails!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqhr7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1aqhaep</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Custom press ons!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my8549bw6iic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1aqfqpx</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Did my own nails using the magnetic velvet effect for the first time!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6o29fyekphic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1aqfgnt</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Spent 6h painting these on myself</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqfgnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1aqfg4h</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Question: Nail techs method of removing acrylics</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqfg4h/question_nail_techs_method_of_removing_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1aqeig1</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Gel x artists what’s ur fav flash cure lamp?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqeig1/gel_x_artists_whats_ur_fav_flash_cure_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1aqe9t0</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Ready for Valentines 💘💃🏻</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hbvn24wahic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1aqe8u4</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Did these myself for the very first time. Honest opinions!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5ga7oylahic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1aqdt9f</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>I painted my MIL’s nails with her favorite NASCAR racecars to gear up for the Daytona 500 this weekend.</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqdt9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1aqdpri</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>This polish has gotten a lot of love from students this week haha. It really is beautiful, in all different lightings ❤️💕</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqdpri</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1aqd416</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>First time done in over a year!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/la86jqz30hic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1aqckh6</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Fresh gel mani!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vb5997h8vgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1aqchak</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Valentine Nails!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucy9quegugic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1aqc8j0</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Help! I've never seen gel polish turn into... Jell-O?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqcmelr9sgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1aqc5pp</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Press on nails come off in shower- replace them all?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqc5pp/press_on_nails_come_off_in_shower_replace_them_all/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1aqc5h9</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Romantic wallpaper vibes</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqc5h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1aqc404</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Cutie floralssss 🌼</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wu2winu5rgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1aqbvnv</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Valentine nails</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e34j7bo3pgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1aqbhms</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Happy V day</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqbhms</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1aqbgiu</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Neon pink for Valentine’s Day 💗 (since they’re not heart themed lol)</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6cdipzflgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1aqbbqd</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>ny gel set i did on myself:)</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4tis1wsakgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1aqb94j</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Shiny pink nails for Valentine’s and my birthday!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30er56apjgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1aqaubc</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Sanrio Dark Valentines Sculpted Nails 🖤</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqaubc</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1aqapc5</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>What’s a good color to get in between Valentine’s Day and St. Patrick’s Day?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqapc5/whats_a_good_color_to_get_in_between_valentines/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1aqaoc8</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I got carried away with the gems</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv8xqxxpegic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1aqaoab</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Told my nail lady I'll be spending Valentines Day alone, she said "Your nails will love you" and added a little heart</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6go5s9pegic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1aq9axj</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Gel X Tips Very Hard to Remove</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aq9axj/gel_x_tips_very_hard_to_remove/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1aq91nv</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>which nails shoe would look best for my hand shape?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl8eles51gic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1aq8qmi</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set💕</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmwb7aruyfic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1aq8nv7</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Chrome and Nail Art</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aq8nv7/chrome_and_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1aq828p</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>First time playing with chrome!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq828p</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1aq7x55</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>First time doing my own nails with extensions + gel!</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq7x55</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1aq7jri</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>help, should i go back to get it fixed?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zow6kzeupfic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1aq4sb8</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Does anyone know the name/website for these press on nails? (see photo attached)</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq4sb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1aq45bo</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Serious question, how do you wash dishes with long nails?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31l2yv9w0fic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1aq37zv</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>BIAB lifting after 2 days?!</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq37zv</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1aq6vsf</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Nail art on my natural nails!</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq6vsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1aq6dok</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Typical Tuesday</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq6dok</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1aq641g</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Hopped on the Valentine’s nails trend</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ew92jg7ffic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1aq5uwp</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Valentine’s themed nails 💓🩷✨ I just like pink and this is a good excuse</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq5uwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1aq5jpk</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Butterflies with pink ombre!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwlu62a1bfic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1aq5ga1</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Valentine's Day nails, by me❤️🔥</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq5ga1</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1aq5cyk</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Am I the only one obsessed about this color?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by2g7imn9fic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1aq4bwd</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Flimsy and thin nails! Help!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aq4bwd/flimsy_and_thin_nails_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1aq44hi</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>A thermal valentines look 💌</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq44hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1aq41vk</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Everything peels off my nails! Please help!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aq41vk/everything_peels_off_my_nails_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1aq3qqa</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Bluey Nails for 4 year olds party</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq3qqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1aq3377</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Red bottoms x french x chrome by me for me</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq3377</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1aq2s1w</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>🍀 ILNP Clover ✨ So juicy and citrusy and sparkly!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq2s1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1aq2kat</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Everything I try fails</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0xgv45gpeic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1aq2is1</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>My nails grow really quickly and love them, but they are very uncomfortable. I let them grow for month before cutting back to my preferred length (before and after)</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq2is1</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1aq0fqc</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>I can’t be the only one…</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aq0fqc/i_cant_be_the_only_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1aq1yz2</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Sassy saints dip kit review</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq1yz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1aq1pjz</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>I tried to match my nails to my ring</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq1pjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1aq119o</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Only using gel base and top coat</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aq119o/only_using_gel_base_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1aq106s</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Nail techs not grinding away natural nail under acrylics?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ao8a6efdeeic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1aq0ftc</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>In vino veritas?</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4kdv07caeic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1aq03k2</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>I'm in love! Can't stop looking at them 💚</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq03k2</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1aq022x</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Valentines press-ons 💗</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq022x</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1aq013x</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Valentine’s Day aura nails</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl00lcah7eic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1apzm0q</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>i really did have a set planned for valentine’s day. i don’t even know what happened 😅</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apzm0q</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1apz7yk</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>How do I grow healthy nails, naturally?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apz7yk/how_do_i_grow_healthy_nails_naturally/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1apzucv</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>my Valentine's day nails done at home!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apzucv</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1apzjgk</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>my favorite 🤩</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apzjgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1apza7n</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>First time playing with magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zin1do82eic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1apz87c</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Help color match!!</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apz87c</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1apyyw3</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Why not go for one design each finger? @kantima salon, bgk</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od4e8ezzzdic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1apyma8</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Missing my long nails rn 😭 curse you guitar</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apyma8</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1apxfq4</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>My nail art vs nail inspo on IG @_beautbybee</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apxfq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1apxbsc</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Help, how do I fix this?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apxbsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1apuso1</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Dip on Cracked/Split Nails?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl2b2iw55dic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1aps9x8</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Does anyone know what is this thing and how am I supposed to use it?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aps9x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1aprlat</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Need suggestions</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7o7g1f9ccic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1appgsi</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Undertone and nail color</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1appgsi/undertone_and_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1apb47j</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Please help me decipher this 😂</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rehorllz7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1apxanx</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Nails for a date</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apxanx</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1apwje0</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Pinky valentine 🌸</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcgqpshnidic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1apwgiw</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Suns out nails out</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5i2uml42idic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1apw147</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Valentines pedi</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apw147</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1apvy29</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Strawberry</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apvy29</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1apvxl6</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>First time painting (all) nails!</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jfb27g5edic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1apuuqm</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Love is in the air 💕</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kmnergm5dic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1apu93m</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>By Vanessa Molina - Dangerous Beauty</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apu93m</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1aptpfu</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Went short and sweet for Valentine's Day ❤️</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mou6mqw6wcic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1apsgk3</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Got my nails done after a longer period of time</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lb70r041lcic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1aprgge</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Any tips.</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkc2l7zsacic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ap7wpc</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Extra big hearts ♥️♥️♥️</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg48gxb2d7ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1apcwx1</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mcmz9plc8ic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1apgted</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Lifelong biter / weak nails after gel extensions</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apgted/lifelong_biter_weak_nails_after_gel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1apkcmk</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Finally!</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71nugzbr1aic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1apq19l</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Natural nails for 3 years strong! (Nail art by me)</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apq19l</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1appxlz</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>These are my favourites so far 🔥</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1appxlz</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1app2uo</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>I think I found my orange? What do you think?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1app2uo</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1apouo1</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Looking for good nail salons in Chicago.</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1apouo1/looking_for_good_nail_salons_in_chicago/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1aqggs7</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Bottle sizes</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqggs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1aqezb8</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Zoya Valentines Gift with Purchase</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aqezb8/zoya_valentines_gift_with_purchase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1aqecmy</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Tried velvet nails for the first time!!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oahq6k3lbhic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1aqdq4w</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>V-day (mighty short) nails 💕</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aqdq4w/vday_mighty_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1aqdka1</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Loving Cirque’s jellies</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ac6bqvad4hic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1aqcp5p</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>A Skittle for all the new polish I wanted to try!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqcp5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1aqbrk9</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Shimmy Shake experimentation</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqbrk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1aqbp1e</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Joined the ilnp fairy dust family 🧚🏻✨</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aqbp1e/joined_the_ilnp_fairy_dust_family/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1aqbo4o</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Thermal formula</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjv930yangic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1aqbgv0</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Third time really is the charm</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7n6027jlgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1aqb7vo</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Mooncat smokescreen :) 💨🔥</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqb7vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1aqaxnu</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>I deem my first try at French tips a success</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pc7q61rxggic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1aqan89</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Funky Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqan89</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1aqacv3</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Lyn B Designs "I'll Never Leave Your Pizza Burning."</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqacv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1aq9eyp</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Matilda</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xfdwzip54gic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1aq9avh</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Does anyone know how I can make these less clear in the middle?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2vr4pd73gic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1aq9052</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>My thumb always bubbles</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq9052</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1aq8znz</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>A fun lil smoosh marble</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq8znz</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1aq8688</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>simple valentines day nails!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq8688</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1aq6j4r</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Sally Hansen dupe that Doesn't smell crazy?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq6j4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1aq79d1</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Blue Lotus 💙😰 Leesha's Lacquer</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq79d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1aq6qrq</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Feeling spicy this week ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq6qrq</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1aq66gi</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Help me can I save her?!😭</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq66gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1aq5nnc</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Another TJMaxx-only Orly?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq5nnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1aq4qv8</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Drip Drop + cat tax</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq4qv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1aq4b6h</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Good or Bad?</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8gi2gh22fic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1aq3zda</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Valentine’s!</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq3zda</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1aq3yss</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Flower French tips for spring 🥰🌸🌼</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq3yss</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1aq3upc</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Valentine's nails</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq3upc</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1aq3uar</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Expressie "trend &amp; snap" for Valentine's Day! ❤️✨</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/se662lsmyeic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1aq31pf</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Chipping within 24-40 hours</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4ki7idvseic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1aq31mu</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Sassy Sauce 4 polishes swatches</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq31mu</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1aq2xd0</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Say Love♥️🤟✨from ILNP</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq2xd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1aq2qf1</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>🍀 ILNP Clover ✨ So juicy and citrusy and sparkly!</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq2qf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1aq2mpf</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Holo Taco Coral Chaser</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq2mpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1aq2izh</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Vertical cat-eye: an underrated magnetization style</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i9lx0t76peic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1aq2h6s</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>My Valentine Press Ons</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsagqxstoeic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1aq0l8d</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Magic Candy</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq0l8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1aq1kz2</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Pink magnetic hearts and velvet nails for Valentine’s Day💕</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cnvtrjcbieic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1aq1jn8</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Summoning Spring 🌱🌸</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq1jn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1aq14gy</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Fox Sparrow + Star Smut (DVN)</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwrw7227feic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1aq0nix</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Lumen - Lethal Lillies</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq0nix</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1aq0n0i</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Golden Child/Problem Child [nails]</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aq0n0i/golden_childproblem_child_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1aq048z</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Do you ever mix your own polishes?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aq048z/do_you_ever_mix_your_own_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1apzvhy</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>there was a valentine’s day plan… idk what happened to it 😅</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apzvhy</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1apzsro</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Obsessed with Death Valley Nails color 'Blue Valentine'!!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apzsro</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1apzgw1</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>I love my new Evil Cyberpunk Vampire nails</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t37xmudj3eic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1apybhs</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Fav top coats</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apybhs/fav_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1apy97f</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Decided after my last post that I'm going to switch back to regular nail polish! Would love to get some colour recs</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apy97f/decided_after_my_last_post_that_im_going_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1apt1lr</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>My Lunar New Year/ Super Bowl Chiefs nails ♥️🐲💛 Polishes Used: Cirque Colors (Shade: 777) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apt1lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1apxj8x</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>2024 Valentine manis</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apxj8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1apx1iq</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovl69ypbmdic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1apx18f</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>does anyone know of any dupes for When Hell Freezes Over by Mooncat?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57s34qd9mdic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1apwxwn</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>What is your favorite glittery pink polish?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apwxwn/what_is_your_favorite_glittery_pink_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1apwbyv</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>It's giving raw hot dogs 😂</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnyh146ygdic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1apvonc</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Recommendation Needed</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apvonc</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1apveu4</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a good dupe! </t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yo61d5q8adic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1apv5bj</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Madam Glam</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apv5bj/madam_glam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1apuswz</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Kissin’ Kate’s Rattlesnake Venom</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apuswz</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1apu72r</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>By Vanessa Molina - Dangerous Beauty</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apu72r</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1apu4sb</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Pink Lemonade !!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apu4sb</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1aptm2r</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>who wants another valentine’s mani?? 🙋‍♀️</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aptm2r</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1apt823</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>This weeks duo ft Cadillacquer and Zombie Claw</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apt823</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1apt62u</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Really basic but I’ve been a chronic biter for years.. grew em out and learned how to do them myself!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q31korfhrcic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1apt2an</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Favourite peel off bases?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1apt2an/favourite_peel_off_bases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1apse8q</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>How are you guys getting such good photos of your glitters?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rurny4lekcic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1aprzl8</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>ILNP Forest Drive has got my heart</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aprzl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1aprgt1</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Does anyone know when the new Lumen collection goes live today?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aprgt1/does_anyone_know_when_the_new_lumen_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1apqyzx</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>I don't know how I feel about this</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjqh298a5cic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1aqgbsk</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>What are some interesting types of nail polish?</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1aqgbsk/what_are_some_interesting_types_of_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1aqg4e9</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>💕💕</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n39cdzmkthic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1aqerst</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>I am a manicurist, in this case my client is called Florencia. She chose a kapping in shades of PINK. They were really very delicate.</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqerst</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1aqeqt8</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>I am a manicurist, and I made these SOFT GEL for my client Mariela. He chose reflective polishes. I really think it was a good choice and good job on my part.</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv8qxtfbfhic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1aqecnf</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>I am a manicurist and in my opinion these were the best SOFT GEL that I did. The right hand was difficult for me to do since I am right-handed.</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qzfao1gbhic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1aqds8l</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>I am a manicurist and I did this work at SOFT GEL today at my location for my client LORENA. I used reflective polishes, they look very beautiful. Constructive criticism is accepted to continue growing</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m365g0o46hic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1aqd8gu</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Magnetic gel on gold people</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ovpvtsg91hic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1aqbwiy</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Valentine nails</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oq8qhngbpgic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1aqbmtz</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Super proud of these! 🪲</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqbmtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1aqavb0</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Dark Valentine’s Sanrio Nails 🖤</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqavb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1aq8b0c</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Fourth Wing Concept Nails - thumb is blue dragon scales. Don’t by my self @jolley.nails</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq8b0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1aq5jbl</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Newest set, done by me ❤️🔥</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq5jbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1aq3v92</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>🐶 valentine nails</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aq3v92</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1aq2szc</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Valentines DYI</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ze9i1y4reic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1aq0q1j</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>My turquoise and shiny nails 🩵💅</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/voudbxsdceic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1apy3ll</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>💖</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/crzi8afwtdic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1apxq6x</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Dry manicure, gel polish and hand painted for mom❤️ What do you think about my work?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3jo2328rdic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1apvzec</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Valentines pedi</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1apvzec</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1aptv2y</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>First try on nail art</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yql9pkgxcic1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Feb 15 08:07:57 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_18.xlsx
+++ b/data/2024_02_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C661"/>
+  <dimension ref="A1:C847"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11670,6 +11670,3168 @@
         </is>
       </c>
     </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1arabxy</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Sakramel nail school - online course in English</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1arabxy/sakramel_nail_school_online_course_in_english/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ar9o0d</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Any good clear polishes?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ar9o0d/any_good_clear_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ar8khf</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Wanted to show off a couple of my favorite sets. My nail tech is my fav🤩</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar8khf</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ar79yk</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Decided to try it for fun, definitely no expert, but Happy Valentine's Day!</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlafq8jzgoic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ar6qdh</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>First set on myself..tips?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5n8q4o0jboic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ar6phw</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Hey💖 I’m a nail tech and would like to show my works🥰</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar6phw</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ar643n</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Practice!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slhbrnve5oic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ar52sn</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Happy Valentines &amp; Singles Awareness Day!😅💘💔 (First time using Apres Gel-X Nails &amp; Solid Gel Glue! Some sizing was wrong but I'm overall happy!! And yes, my right thumb is way shorter...I'm a gamer and my gaming mmo mouse has 12 buttons on the side that I can only push if my nail is short!😆)</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p96ps695vnic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ar496a</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails!</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar496a</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ar3sxu</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Valentine's Press On Nails I made &amp; with the flowers my bf arranged 🥹💝✨</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/26bop8x0knic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ar3pux</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Should I have done a different color tip?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of4tje8ajnic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ar3og5</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>I 💝 stamping and I’m totally not salty about a recent breakup</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar3og5</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ar3ddi</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Happy Valentines 💖</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar3ddi</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ar25y7</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Acrylic or liquid gel???</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ar25y7/acrylic_or_liquid_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ar25ao</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Valentines nails ❤️</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar25ao</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ar1do7</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>My valentine’s day ❤️</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar1do7</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ar171u</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Kiss Salon Design in Nailed It</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df7uwltpymic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ar0mtq</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Happy Galentine’s Day!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9xbwkscumic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1ar0ex8</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day 💖🖤</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar0ex8</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ar010g</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day 💕</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar010g</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1ar005t</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Who doesn’t love valentines nails and cute little fuzzy noses! ::boop:: Happy Valentines Day!</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n693ocaepmic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1aqzqkh</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Love Letter Nails</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78kki3tummic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1aqziay</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>What do you think of these?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ai5o8wamlmic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1aqyzia</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Happy valentines ❤️</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5g39tzphmic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1aqyiix</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Just got done with my right hand. Placing charms is so hard!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5s69a54emic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1aqxoxs</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69tmq9os7mic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1aqqzno</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqqzno</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1aqxzsx</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Starting my nail journey! Which shapes would you recommend?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqxzsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1aqxsdx</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>My fave set ever</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqxsdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1aqxi4q</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>I need your advice/troubleshooting about soak-removing hybrid gel nails.</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqxi4q/i_need_your_advicetroubleshooting_about/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1aqxgei</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Hand painted swan set for Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqxgei</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1aqxaei</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set I did last night!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqxaei</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1aqx0i2</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>With love🤍</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p37871do2mic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1aqwxt3</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Searching for the best pink shade for my hands. Have I finally nailed it? 🤍 ʚ(* ´꒳` *)ɞ</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqwxt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1aqwtbc</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Valentines nails💕</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw5pudc61mic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1aqvd2x</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>My press on nails I created some bubbles but still love them</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nij9y1lgqlic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1aquh9x</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Semi cured gel strips are just not adhering to my nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aquh9x/semi_cured_gel_strips_are_just_not_adhering_to_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1aquh5j</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Love or hate?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aquh5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1aqu8df</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Valentine's Day set I did last night!</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqu8df</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1aqu66z</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>did these on myself! self taught using polygel for almost 5 years</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ixm5gax0ilic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1aqu43c</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Anti-pink Valentine’s Day set</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ht0jb8phlic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1aqt5vx</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Vegas nails for Saturday! 💅🏻</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqt5vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1aqsyv4</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Valentine’s nails, even if I’m hopelessly single</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqsyv4</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1aqsw24</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Happy Valentines Day! ❤️🌹</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6x43voy8lic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1aqsgih</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>I wanted to join the valentine’s theme ❤️</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clc5x11t5lic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1aqsfsy</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails :)</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqsfsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1aqs3vg</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>His and Hers Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqs3vg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1aqrl0u</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>How to recreate this on nails?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qc7t3h9izkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1aqrdsf</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Thick and dry cuticles no matter what I do</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz9clki2ykic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1aqqz6s</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day 💝</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czd7dq23vkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1aqqs3g</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Wedding nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqqs3g/wedding_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1aqqhqb</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>My favorite thing is when my toes match my hands eee</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/210tmgkgrkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1aqq4s5</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Subtle Valentine's nails, full coverage tips hand painted by yours truly xoxo</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqq4s5</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1aqopjm</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Valentines nails ❤️</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1rdblq4ekic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1aqoo05</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqoo05/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1aqq252</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Guys I'm like 98% sure I just did my engagement nails</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6g3dduw9okic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1aqq1mh</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slmidyo5okic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1aqptlp</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Did my nails for Valentine's Day!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqptlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1aqpsgs</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Nothing too fancy, but wanted to see how I liked this new gold color I bought</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sut2ewr9mkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1aqpntb</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>🤍🎀</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lowd9walkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1aqpk60</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Best quality/price products that can be purchased wholesale from china?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqpk60/best_qualityprice_products_that_can_be_purchased/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1aqpk1q</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>My boyfriend is planning to propose soon! What are some neutral colors I can look at that will look elegant but let the ring shine? Hoping they grow out enough so I can do almond shape</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8hk508kkkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1aqpcyg</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Happy Love Day!</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqpcyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1aqp5e2</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Nude rubber base &amp; sheer white</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6xanb1hhkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1aqogv2</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Galaxy Nails</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qz2uqwl6ckic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1aqoax2</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>New nails for Valentine's Day 🥰</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmjmhplxakic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1aqntj5</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Lateral nail folds?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqntj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1aqnjjb</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Valentine’s Day new nails 💜💫✨</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cks969r4kic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1aqnd6g</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Happy Valentine's day</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqnd6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1aqn6aw</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Is liquid gel extensions a thing?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aqn6aw/is_liquid_gel_extensions_a_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1aqm0xs</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Valentine's nails 💖🔪</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqm0xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1aqlv7x</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Opinion on nail shape?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvhhcf9mpjic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1aqlep8</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Sweet and Sour Lacquer - Shits and Giggles 💩😃</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqlep8</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1aqkxu7</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>All ready for valentine's day.</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx9reaj0gjic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1aqkdf7</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Simple but classic</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqkdf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1aqjksx</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Happy Normal Wednesday to all of us single people 🖤</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hikeb590jic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1aqj8tw</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>valentine’s day nails 💕</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kudzen74wiic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1aqi43m</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>happy valentine’s day! 🩷</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqi43m</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1aqhzir</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Natural nails with gelpolish 💋</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfq4a7akfiic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1ar9iow</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>My French always goes wrong!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dir62czn5pic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1ar72fv</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Mooncat Pumpkin King with matte topcoat</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v66ynnwxeoic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1ar70p4</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Velvet Valentine 🎀💖</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/opk5mkg8eoic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1ar6r1j</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Gelike EC</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar6r1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1ar68x4</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day!</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3bsei6q6oic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1ar5sru</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>This color tho.. 🐍</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lzpx1dnb2oic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1ar5r3z</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Can someone help me find a dupe for Zoya Tracie?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ar5r3z/can_someone_help_me_find_a_dupe_for_zoya_tracie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1ar0jyt</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Be Mine by „Isle and Pea“ for Valentine‘s Day</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar0jyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1ar54ex</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>London town reviews?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ar54ex/london_town_reviews/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1ar4hhc</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Lazy Valentine’s Day nails</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wckbda6qnic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1ar3xam</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Favorite one coats</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ar3xam/favorite_one_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1ar3ozl</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>What are your favourite Polish Brands?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ar3ozl/what_are_your_favourite_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1ar3eml</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>I'm in love with this polish, so happy valentine's to her</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar3eml</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1ar2lbw</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>New colors!!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar2lbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1ar2ika</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>OPI - Angels Flight to Starry Nights (again)</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l27hpwh09nic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1ar2dpz</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>My valentines nails ❤️</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar2dpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1ar2bof</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Death Valley Celestine</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar2bof</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1ar1psv</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I LOVE THERMALS. That is all</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw3zeofp2nic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1ar0s90</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Fair Maiden Moonstone Magic</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar0s90</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1ar0rnp</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Wild and Mild (European brand) Pretty Promise</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0cok3grevmic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1ar0eu8</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>I wanted to do Valentine's nails toooo</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar0eu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1ar0c4v</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Now that Valentine's Day is over, what's next?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar0c4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1ar02pv</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day❣️I am OBSESSED with this polish!!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar02pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1aqzid0</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Holographic Pink - ILNP Flower Girl</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqzid0</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1aqzhy9</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Easier than expected heart nail art!!</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb8vzhsjlmic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1aqzhno</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>valentines mani</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2twxgahhlmic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1aqxp9q</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>What yellow will fit in here?</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqxp9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1aqxbpl</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>First thermal polish for V day</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqxbpl</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1aqx83a</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>A *little* stamping for V-Day ✨️</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqx83a</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1aqwyt9</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>February manis so far… keep scrolling if you’re sick of pink 😅</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqwyt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1aqwszy</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Pink skittle mani bc 'tis the season aka trying out half of my 1st ILNP order</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqwszy</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1aqwsv8</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Valentines Day with my first ever PPU order!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqwsv8</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1aqwpjh</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Clionadh- Heart of fallen star</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqwpjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1aqwijr</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>first time trying to do hearts &lt;3</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dbk7rewylic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1aqwiip</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Kathleen and Co - Rosary Pea</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqwiip</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1aqwgmk</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>my dream valentine’s skittle 💓</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqwgmk</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1aqvxns</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Groovy polka-dot Valentines</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqvxns</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1aqvrmi</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Ether Dragon (pics 1&amp;2) &amp; Glass Jellyfish (3&amp;4) layered on top of ILNP Pine creme</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqvrmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1aqvblg</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Pink Valentine Mani. Modelones #0905</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77w3nlc5qlic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1aqv427</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Valentine’s Day linear holo skittle</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqv427</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1aqv1ui</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Was going for a gas station gift look for V-Day</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqv1ui</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1aquois</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Love at Frost Sight</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ky3zz9nllic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1aquklo</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>A Kiss for Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2c2fijnklic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1aqu9xg</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Top coat with no discoloration?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aqu9xg/top_coat_with_no_discoloration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1aqu4x3</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Inlp poppy for Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/df3uclsuhlic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1aqu3jh</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Let’s see your Valentine’s nails! I’ll start</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w03qqykhlic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1aqtzme</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/384et6dtglic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1aqtn51</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Matte winter manicure ❄️</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyovhazcelic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1aqrsaw</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>ILNP - 1Up</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/opbputdx0lic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1aqrovx</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Rosary Pea!</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqrovx</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1aqrm60</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Why are my nails so flexible?</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mbjjqzxizkic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1aqr6cs</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>My most fancy Valentine’s nails ever</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9uqypmjwkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1aqqvzy</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Boolba over Cirque Colors Organza</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqqvzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1aqqupc</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Mooncat- Mercury Tears</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqu0ctw4ukic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1aqqtp8</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Valentine's hearts</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqqtp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1aqq9io</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Swamp Gloss Feed Me!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzo4hjwtpkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1aqq43l</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Distracting AF!</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9bin7evnokic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1aqq3eu</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Water marble heart 💕</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8qrgv4jokic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1aqptwy</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Il(Lūmen)nation</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4nvovogmkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1aqpsrv</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Did my nails for Valentine's Day! 💖</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqpsrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1aqpngt</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Blood Moon by Mooncat in the sun is giving me life</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/334c9th7lkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1aqpmy0</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>valentines holo mani of my dreams 🤩</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqpmy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1aqpkrd</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Magnet question</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aqpkrd/magnet_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1aqp4r7</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>my little chocolate covered strawberry buddies. nom nom</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqp4r7</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1aqp3du</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Black &amp; Green &amp; Gold</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbzo7e22hkic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1aqonux</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Happy Valentines Day!</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snt968kqdkic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1aqom8g</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Cold black heart</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqom8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1aqobq1</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Valentine’s nails (after and before)</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqobq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1aqo1w5</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day, nail buddies!</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqo1w5</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1aqnnqe</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>stamping help?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aqnnqe/stamping_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1aqnnky</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Subtle Valentine's nails 🩷</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqnnky</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1aqmo70</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>'Miss Smoo' Blue</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/x4prRtS</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1aqm9uf</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Gothy Valentines Day</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqm9uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1aqltrc</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Here for the Boos (is it Halloween yet?)</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uoy51ucvojic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1aqlkux</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>This photo. 😍</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4joty4smjic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1aqlgks</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Vampy Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqw3vlkjljic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1aqlfum</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Sweet and Sour Lacquer - Shits and Giggles 💩😃</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqlfum</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1aql5fy</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>First time posting! :)</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz7lisidijic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1aqk6jz</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>I love this pink</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lwx96si7jic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1aqjlia</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Happy Normal Wednesday to all of us single people ❤️</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnim41qh0jic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1aqjjuc</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Simple valentine’s</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqjjuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1aqj2u1</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Would Russian/E-file manicure training courses online be effective?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aqj2u1/would_russianefile_manicure_training_courses/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1aqi7ge</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Looking for dupes (more details in the text part)</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqi7ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1aqi76h</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Valentine Nails 🩷💜</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p0v3al8iiic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1aqhvwk</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Chrome Powder</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/meoa8ulaeiic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1arae2k</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Help me!! (Metallic gel)</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arae2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1ar8iuj</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Finished another care bear 😄 only one more to be painted🥰</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i6c86i6cuoic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1ar78w8</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I’m a manicure and she’s my client Stephie. Look at the beautiful nail art of good quality after a month of growth. Beautiful her nails</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar78w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1ar65el</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Soy manicura y Este Nail Art que es una locura se lo hice a mi clienta Florencia . Las líneas son difíciles</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar65el</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1ar5w7w</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Lunar new year and Valentines Nails, tutorial coming soon!</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gs9ro8qx2oic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1ar5d16</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Labradorite Nails</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y0cbea8ynic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1ar3u5d</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Valentine's Press On Nails I made &amp; with the flowers my bf arranged 🥹💝✨</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oerzgshbknic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1ar3gj4</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails ❤️</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar3gj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1ar065a</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>valentines day nails</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/566ulyipqmic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1aqya0h</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Second set of nails, opinions?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqya0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1aqy0t0</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Purple Abalone 🦪🐚💜✨</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqy0t0</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1aqvi5p</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Strawbeary Valentine's nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqxxf8uirlic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1aquuxy</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>The heart is my favorite 🥰 nails for my client today</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9m4x4e6umlic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1aqujb0</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>What I’m currently working on 💕</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8h8gbqnklic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1aqu49o</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>14 days of Valentines nail art</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqu49o</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1aqt73i</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>I'm actually proud of these!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqw4hr77blic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1aqru0a</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Be My Valentine 💝</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqru0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1aqpbwb</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>nom nom nom</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqpbwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1aqp43m</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>happy valentine’s day!</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqp43m</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1aqnrd4</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Valentine’s Press On’s ❤️</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqnrd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1aqlvs3</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>I’m a manicure, and this hands-on job was for my client Paula who went on vacation to the beach.</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqlvs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1aqia5w</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Barbie Valentine’s</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqia5w</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Feb 16 08:08:05 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_18.xlsx
+++ b/data/2024_02_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C847"/>
+  <dimension ref="A1:C1013"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14832,6 +14832,2828 @@
         </is>
       </c>
     </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1as2wnm</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Clean and simple</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nstlcqxgwic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1as2lpl</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Glass nails 💅</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvom3ec9dwic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1armdri</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>What is your favorite at home manicure method?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1armdri/what_is_your_favorite_at_home_manicure_method/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1arkrjl</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Spooky ocean inspired</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arkrjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1as1jns</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>should I get a fill or a whole new set?it’s about a $20 diff</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r02s6n6j1wic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1as13qg</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>my current set</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hk6s470ywvic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1as10kd</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>First attempt at GelX</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vah31ak0wvic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1as0c4g</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>I just want to know how healthy my nails are and some tips on how to make them grow faster plus a pic of my cat</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as0c4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1as0ao9</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Nail polish always pops off!!!</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00j36z02pvic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1as0amb</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Valentines Set 💕💓💖💘🌸💐🌺</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zurv5p1pvic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1as0afv</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Aurora coating on nude base is gorgeous!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as0afv</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1arzkbw</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cns5tejxhvic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1arziga</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>My first russian manicure! Obsessed!!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bcplh2xfhvic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1arz69e</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Traumatic Static</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arz69e</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1arz0ig</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>In love with this polish color but just ran out🥲</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arz0ig</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1aryiwy</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Got my nails done today, it’s been years since I have! The purple is tiger eye gel paint 💜</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aryiwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1ary1ox</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>a grey overcast day but they still pop 🥰</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ary1ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1arxztk</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>happy belated valentine’s day&lt;3</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arxztk</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1arxn0j</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Red in love</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arxn0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1arxep3</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>What do base and top coats do?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1arxep3/what_do_base_and_top_coats_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1arwo4n</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Fresh set! Asked for something orange</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arwo4n</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1arwfgv</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Press-On Nails 4 Ever 💖</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arwfgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1arw85z</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I call this the clinically clean manicure 💅🏻 </t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wm64qkvxnuic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1arw4vv</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Dry manicure/pedicure experiences?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1arw4vv/dry_manicurepedicure_experiences/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1arw3qo</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Simple studio ghibli nails 🖤</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5kilekwmuic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1arw00c</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>All my nails broke 🥲</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4teh0ttzluic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1arvzml</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in forever. They're kinda extra but I love them! Think strawberry milkshake-vibes 🍓</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arvzml</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1aruome</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Holographic ombre my beloved 😍💋💋</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aruome</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1aruksr</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>and for today a basic orange..🦊🧡</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1j5s6972auic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1artumh</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Got another fake nail set recently for Valentine's day and I AM OBSESSED with how they look!</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6pd4s674uic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1artr6c</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>does this color suit me?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuwyl37l3uic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1artivs</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Romantic green</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1artivs</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1artcw9</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>I’m in LOVE with this cat eye color ! Especially on long coffin</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1artcw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1arszsk</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Dita Von Teese nails</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ajlu3wtxtic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1arsvir</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>First time using the pearl shimmer powder… I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxq3ow1ywtic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1arshhm</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>current set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma489ga2utic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1arsh00</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Nails I got recently</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb9fb11zttic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1arsd5a</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Feeling cute, won’t delete later 💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sh5pxn76ttic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1arsajp</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done yesterday and they put so much topcoat over the jewel that it looks like an egg. Can it be fixed? </t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp1j6ewnstic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1ars6cr</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>What can I charge for this biab/ hard gel overlay + e-manicure?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fup1o2trtic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1arridv</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Nails are growing out. I’m going to add a *little* bit of length. What shape would look good on me?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz9ncq5zmtic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1arqwm2</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>What now?</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6xdcfsmitic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1arqk6p</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Gel or lacquer?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1arqk6p/gel_or_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1arqhtu</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>New set! love them!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arqhtu</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1arqhib</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>My attempt to cover up the indentations, tech went a little heavy handed on my cuticles. Any advices on hiding/healing them?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arqhib</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1arqea3</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hello! I tried hybrid on myself for the first time (simple since I have only one nail polish now..) - any feedback appreciated </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b94rhnfxetic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1arpz2d</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>did my own nails for valentines</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arpz2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1arpkfr</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Gel nails</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1arpkfr/gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1arpdw1</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Nail care tips? I’ve explained more in the caption</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo2spc7l7tic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1arowjj</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>New self mani today</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arowjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1aror6v</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Sparkly blue</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/534ghw7y2tic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1arnygy</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Got my nails done for my birthday ☺️</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arnygy</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1arnva1</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Aspiring nail tech. Looking for tips, tricks, or your come up story💗</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1arnva1/aspiring_nail_tech_looking_for_tips_tricks_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1arnnaz</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Berry 🍓</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwcxoymxusic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1arnmp0</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe7geawsusic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1arnah8</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>what to do with this mess</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arnah8</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1arn750</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>how do we feel about these?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arn750</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1armtj9</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Throwback to my fall nails</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jwdiytrosic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1armqku</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Best Glass File</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1armqku/best_glass_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1armezo</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Any tips for mediating a terrible nail color?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3erwisrlsic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1arm1x8</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Is it too much?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xrhn6d4jsic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1arl988</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Just removed my polish</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhlabs2gdsic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1arkx9l</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Tried something new! (Natural nails, acrylic overlay)</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n9te5i1bsic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1ark5w7</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>I know the day has passed but I wanted to showcase my latest Valentine themed set (my first time getting gel X)</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d64m6t6j5sic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1ark35g</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Now how exactly am I supposed to fix this nail?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3durvty4sic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1arhaya</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Has anyone else not gotten used to nails?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1arhaya/has_anyone_else_not_gotten_used_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1arjpq5</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Lovely black nails with Kuromi</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arjpq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1ardkfm</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>So bad…Please advise</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vplukvqkqic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1arcg7x</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>What have I just bought? Temu nail clippers came with so many things I have no idea what they are meant for.</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cfrmdy27qic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1arjmxr</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>How pretty is the deep french 👌</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxtr5szl1sic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1arca0i</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Sad nails</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g29w55fv4qic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1arjlz1</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>valentine's day set! this was like $15</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arjlz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1arjges</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Look at that color combination! Don't you think she's really beautiful?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xodjygo80sic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1ar7xqq</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>This isn’t normal right? How do I fix this?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/407n0huunoic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1ar6exv</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail glue recommendations </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ar6exv/nail_glue_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1ar4znu</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Nail inspo from the @therudiberry x getquickies collab on ig. Any ideas on how to get this effect?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m03fvsjqunic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1ar435t</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>What is wrong with my nails and how can I get it corrected on my next fill.</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ar435t</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1aqysv5</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day 💞</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aqysv5</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1ariprm</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Do these two go?🩵🤎</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ariprm</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1arijz6</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Belated Happy Valentines day!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arijz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1ariiik</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>I don’t often do my nails, but this was one of my fav nail colors. I like the sheer color</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vg9ocuw9tric1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1ari4gm</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Miss my longer nails, thinking of growing them out again like this</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ari4gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1ari25h</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best nude, pinky nude or light pink for fair skin with rosy/neutral undertones? I don’t want them to blend in or make may fair skin look more pink if that makes sense! I want it to stand out a little bit still neutral… TIA </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ari25h/best_nude_pinky_nude_or_light_pink_for_fair_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1arhpgo</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej5qyeg3nric1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1arhmmm</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Pretty Nails</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v58i9ewhmric1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1arhdep</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>My DIY Nails (PH)</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arhdep</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1argj4l</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Just finished my carebear nail set 🥰✨ who's your fav? ☺️</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1argj4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1arghdk</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Nail care.</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arghdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1arfdo3</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>I want to go back to that color</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g0c4oulbvqic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1arf8ty</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Black and pink</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arf8ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1arf8b9</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>A quick one before I move again 💅✨</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arf8b9</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1aresly</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Beautiful!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nidpbj0yqic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1arelol</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Nails of the week</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arelol</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1ared82</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>How do y’all put on necklaces with nails??</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ared82/how_do_yall_put_on_necklaces_with_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1arecc1</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set done by nail tech 💖</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfiqts9ctqic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1are7b3</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Took my husband for a Valentine's manicure and I'm seriously impressed with the colour he chose 😍</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1p4gthdtrqic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1are4r6</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>did them myself! any feedback? and design ideas because i want to decorate them :)</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1are4r6</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ard8fe</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>French never goes out of style 🤍</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/paifihwtgqic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ard3j8</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>New color</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ard3j8</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1arcdeh</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Which shape suits me better?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arcdeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1as1sru</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>spots in thumb nail</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as1sru</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1as1mad</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Pink!</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as1mad</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1as1bnf</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Death Valley Nails Two Ticks and No Dog</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as1bnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1as113k</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Import stash to lacquergram?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1as113k/import_stash_to_lacquergram/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1as0rpn</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Mooncat Moonrise 💕</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc1mjy2ktvic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1arx2tv</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>My natural nail progress. I know they’re not that long, but I’ve never been able to grow out my nails due to splitting and peeling. Enter builder gel. I can’t believe these are my nails!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43824kd4vuic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1arz60s</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>ordered mooncat polishes and wasn't notified of delivery</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arz60s/ordered_mooncat_polishes_and_wasnt_notified_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1arz4r7</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Hey it matches my chocolate bar!</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arz4r7</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1arz3p8</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish - Traumatic Static</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arz3p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1arysxi</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Love Spell 🪄💘</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arysxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1aryfv9</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Polish to match my engagement ring?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4w8av497vic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ary8xb</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Nail advice - asking the experts!</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ary8xb</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1arwske</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>I'm on the hunt for vibrant non pastel neons. This green isn't quite what I'm looking for but I like it none the less.</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arwske</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1arwdgh</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Can you magnetize magnetic polish too long (velvet style)?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arwdgh/can_you_magnetize_magnetic_polish_too_long_velvet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1arw7eq</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Mood Pebbles</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arw7eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1arvryh</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Pink coquette nails 🎀✨🩷</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7znkoqr1kuic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1arviyl</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Help me find this color 👀</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ow6v9u5xhuic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1arup0u</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arup0u/night_owl_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1arun5q</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Broken nail with gel manicure</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arun5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1aru116</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Sometimes you gotta start over again, that's just life!!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfzpoo7q5uic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1arst1n</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Flicker - INLP</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arst1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1arsip4</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>wedding nails</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru9lr2zbutic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1arshg0</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>God of Idiocy 🥹 + a question</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arshg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ars52f</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>My favorite go-to mani. I call it a double reverse gradient dotticure. What's you're favorite easier-than-it-looks mani?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fth6dzkjrtic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1arryuo</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Another valentines mani 🍫</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arryuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1arrve4</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>OPI - Suzi Takes A Sound Bath</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arrve4</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1arru1l</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse 🌙✨</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfhicav9ptic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1arrrkv</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a sheer pink pearlescent or iridescent shade! </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arrrkv/looking_for_a_sheer_pink_pearlescent_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1arqjd4</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>I need a swatch comparison!!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arqjd4/i_need_a_swatch_comparison/</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1aron10</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Shoutout to everyone who recommended the Canadian brand BKIND 💜 This was so lovely to apply!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8frx6ec62tic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1aroehb</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Valentine's Day Skittle (plus terrible first attempt)</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aroehb</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1arnz2x</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Monarch’s Belladonna</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arnz2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1arnc8c</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Mani #5(?)... grey is a neutral!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arnc8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1armz06</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>First time painting French tips!</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1armz06</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1armsx9</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Hidden Treasure</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1armsx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1arme54</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>When the sun hits 🌈</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4ogor2mlsic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1arlymt</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>This week’s Valentine’s mani 💕</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arlymt</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1arlyhn</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Ridge filler?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arlyhn/ridge_filler/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1arlbrs</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>you. guys.</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arlbrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1arkpf7</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Opinions on Mia Secret Xtrabond Primer?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arkpf7/opinions_on_mia_secret_xtrabond_primer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1arlafw</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Valentine‘s Overcast Skittle Nails ☁️</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arlafw</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1arkrat</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Green 💚</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q1z08bt9sic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1arkj29</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Short Milky White</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b92mufj48sic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1arkent</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Okay Lumen, we get it, you like Mystery Bundles</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1arkent/okay_lumen_we_get_it_you_like_mystery_bundles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ark4f2</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Violet Valentines</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ark4f2</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ark40j</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Hydrangea 💙💜</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ark40j</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1arjtxg</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Not the best background, but here's Written Invitation, Emily De Molly</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arjtxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1arjrqe</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can’t stop staring at these </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0fg1q5ek2sic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1areylq</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Happy Valentine’s Day 🩷 Polishes Used: By Dany Vianna (Shade: Pink Is For…) | Essie (Shade: Gel Couture Top Coat)</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1areylq</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1arhwnw</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Lovebomb 🥀</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arhwnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1aremib</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Cock-A-Doodle-Doom by Sassy Sauce</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aremib</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ard6yh</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>New color</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ard6yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1as38gp</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Hand painted modern art with classic primary colour pallet on Gel nails.</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as38gp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1as0uvh</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Cinderella Movie Nails</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as0uvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1as099l</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Nude base with aurora coating!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as099l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1arzwm9</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Valentines Day Set. (Even though I'm late)</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arzwm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1arz310</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>My Valentines Nails 💞</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4d1n8ewbdvic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1arx9g7</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>[Better picture] Whatyl would help me improve my Monet watercolor look?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arx9g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1arx68j</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>What could help me improve my Monet look?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arx68j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1arvscj</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Wanted to share this press on set I finished last night!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgk7cbi5kuic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1artuqs</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>I unintentionally matched my nails to my favorite scrunchie.</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2g2g31fb4uic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1armxet</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>How can I fix that</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1armxet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1arjo4e</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Just did these for Date Night</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arjo4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1argjkd</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Just finished my carebear nail set 🥰✨ who's your fav? ☺️</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1argjkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1arcgqg</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Futurama Nails</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg2kyok97qic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1arc4lr</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Newly made press ons (handpainted by me)</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arc4lr</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Feb 17 08:07:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_18.xlsx
+++ b/data/2024_02_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1013"/>
+  <dimension ref="A1:C1155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17654,6 +17654,2420 @@
         </is>
       </c>
     </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1aswr54</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>My 2yo said "oooh, I like them" 💕</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aswr54</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1aswcpw</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I found my forever nail girl😩 Been staring at this catching the light all day! Jelly + cat eye gel on my natural nails.</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b1le96p6m3jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1aswagc</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>My Valentine’s Day not so Valentine’s Day nails is my only obsession right now 😩😻</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aswagc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1asvonj</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>My nails for valentines. I tried my best.</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bccffxwke3jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1asuspo</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Nail appointments are my fav 😊</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqhjieru43jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1asud6v</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>New Spring Set</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqkm95ge03jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1asu1zx</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>fav set💕</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m7vxlx97x2jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1astlwq</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Hand sculpted custom sanrio at the fair press ons by me! 🎠</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1astlwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1asti1a</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>2nd polygel attempt</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asti1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1asteof</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>press ons I made</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpefn2uoq2jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ast5qe</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>My nail tech always gets me right&lt;3</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vs8pbfhao2jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1ast2vm</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>First time using builder gel</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kt4q71zin2jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1assf8k</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Hard gel is hard!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1assf8k/hard_gel_is_hard/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1asshf8</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to prevent nail chipping/peeling? </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asshf8/how_to_prevent_nail_chippingpeeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1aslrfu</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Nail Salon Didn’t Finish Curing My Nails</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aslrfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1asn74z</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Gel x</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asn74z/gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1asnmdc</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Lace Nails! In honor of Stevie Nicks' Leather &amp; Lace</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asnmdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1assgef</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>What am I doing wrong to cause this weird curve on the underside of some of my nails? Second pic is how most of them are, much straighter. I use tips</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1assgef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1askrp8</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Please help a newbie</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1askrp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1asmqlh</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Feel like my regular nail tech would've ATE this look 😒</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk0dlvhv51jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1aso2o2</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Allergies</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aso2o2/allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ass6n4</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>They looked better in my head</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dicf6pt4f2jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1asrssc</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Love day nails 🩷</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03x8qvkkb2jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1asr0ca</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4drcijgj42jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1asqe3r</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting gel nails removed </t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asqe3r/getting_gel_nails_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1asqbya</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>just got these done 🥰 a little longer + brighter than I usually get but baby pink chrome!</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asqbya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1aspu7t</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Calling this a subtle grape milk ombré 🥛🍇</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uo2sciju1jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1asot9s</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>these are my nails for vday 🩷</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plamsqu3m1jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1asoi8i</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>My friend does my nails and played with a new white chrome powder. Didn’t turn out as expected, but kind of loving the surprise soft velvet look!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asoi8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1asnu54</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Kirby nailsss</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isxyqm3be1jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1asn6d5</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>A simple but cute design! ☺️</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c71k1dq891jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1asmtsz</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Going to will summer into existence</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asmtsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1aslikg</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Salon filled gel in with acrylic and my anxiety is running wild </t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aslikg/help_salon_filled_gel_in_with_acrylic_and_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1askqpv</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>How can I fix cracked nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0nbhhguq0jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ask3v7</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Fresh Manicure</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ask3v7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1asexqd</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Need a rec for builder gel</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asexqd/need_a_rec_for_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1aslkjb</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Safe to do gel?</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lmxz4vyw0jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1aslh3q</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>How can i fix this nail?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4s8399aw0jc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1aslcs4</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Pink and dandelion set</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aslcs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1asl6qc</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Accidental Ukrainian flag😅 🇺🇦</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asl6qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1askcax</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Went back to my old ways</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipu69fewn0jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1asjmse</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Charms is definitely my new favorite thing!</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzr7gjani0jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1asj9ta</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Zero Gel Polish</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asj9ta/zero_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1asiuua</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hey girls 💕 I didn’t do my nails for a while and I decided to come back with something reliable! </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6y3p067zc0jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1asi8nu</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Nail tool sanitizing?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asi8nu/nail_tool_sanitizing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ashy3o</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry red 🍒 </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/moet3mvb60jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ashnqe</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>February Nails🩷</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ashnqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1asgpe6</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>I could kill a weaker man with my thumbnail</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asgpe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1asgonl</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>my first biab set</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asgonl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1asgnea</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Got my first ever manicure, am I wrong to be a bit disappointed? Polish doesn't even go all the way to the edge of my nail or over the tip.</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asgnea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1asg64l</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>may have found the perfect red?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asg64l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1asfgdu</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Genital nails for Valentine's day </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wyyrf25ynzic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1asfbz2</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>First time doing my own nails (poly gel)</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn8b49w1nzic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1asf6as</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>🌊🪨🔥💨</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/olmjap3xlzic1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1asexjq</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Removing cuticles with oil</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asexjq/removing_cuticles_with_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1asedzl</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>For the month of love ❤️</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asedzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ase267</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>🔥</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/309eh0w3ezic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1asd7x4</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Beige with hints of green sparkle</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3tb7gp28zic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1asb4pw</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>LNY/ Valentines Nails!</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asb4pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1as9til</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>How long between fills?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as9til</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1as7vp6</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>how do I fix this???</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as7vp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1as793m</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regular nail polish instead of gel </t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1as793m/regular_nail_polish_instead_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1as6yyi</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>accidentally cut my nail plate. What do I do?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccu60nuptxic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1arywit</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Nail has a bump - does anyone know what it is?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arywit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1arxs2e</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Are those air pockets?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1arxs2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1asbz7d</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>MY PHOTO</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fr4bwun6zyic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1artnx4</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Beginner at Acrylics: How do I make them last longer?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhpm2hqw2uic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1asb0z2</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Red velvet for February ♥️</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asb0z2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1asayfu</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Is it okay to get a manicure with bitten and sometimes bleeding nails?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1asayfu/is_it_okay_to_get_a_manicure_with_bitten_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1asaszs</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Attempt at doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxnvnmrdqyic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1asak41</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>I did subtle post valentines day nails 💌 ❤️</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asak41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1asa4ae</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Are these oval shaped ?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asa4ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1as9oq2</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I'm happy to have achieved this design❤️</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s97jp6yhyic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1as9mit</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>I wasn't ready to look at my nails every 10 minutes.</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ai4mrhhhyic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1as861z</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Love the Color</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8kmr4y55yic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1as7xkx</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I really like this set</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as7xkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1as7plb</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Sparkly violet. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as7plb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1as75ci</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>I’m blue dabadedabadi</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo0v3mojvxic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1as743x</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>First time getting my nails done! It feels weird but I love it ❤️</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as743x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1as5jqu</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Square or almond?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as5jqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1as58ay</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Starlight so bright</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as58ay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1as4r5n</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Some simple nailsets that I made today / short oval shape / short coffin shape / short oval shape</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as4r5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1as3p83</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Blue wedding (bride) nails</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as3p83</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1asv9ky</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Cirque - Aegean</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asv9ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1asuxr0</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>One of these does not belong</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dn1atxp963jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1astm4z</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Simplicity</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1astm4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1astbru</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Polished for Days Angel Wings</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1astbru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ast0yt</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>After 10 days</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv4525uzm2jc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ass8wh</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>How do you get this effect / design?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxgeznbqf2jc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ass31t</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Cupcake Polish- La Lluvia</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6y4qv5h6e2jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1asrif9</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>February Mani #6...orangey???</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asrif9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1asqwc9</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Dragon eggs…but make it teal!</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1lk6jpi32jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1asqtxc</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Finally bought a magnetic polish……and oh my…..,</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m41u4vgx22jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1asqpb4</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>ILNP Bishop</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asqpb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1asqit3</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Best reflective walking gear</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jzv84vb02jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1aspx7d</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Toppers/special effect polish swatches</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aspx7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1asnvay</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Nail clean up brush</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1asnvay/nail_clean_up_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1asmsm0</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>First attempt at nail art!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asmsm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1asmslx</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>ILNP ‘Ariel’ 😍❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asmslx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1asmckz</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>ILNP Shooting Star</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdfsiddv21jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1asmany</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>How can I improve these?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwld866d21jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1asknjl</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>House of Winter? Hades Blues?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asknjl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1asjzlf</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>heat transfer nails 💅</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asjzlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1asjzk8</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Flight of the Monarchs feat. lobster Bisque</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76mogvb9l0jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1asjho4</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Absolutely in love with this combo</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asjho4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1asiyr9</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Bloomin' marvellous 🌷</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/zbaul7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ashq81</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Is it green? Is it blue?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ashq81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1ashnfd</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Is green my color?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6mblpwb340jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1asheww</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Public bathroom matching perfectly</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlc4oz8b20jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ashdmj</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Princess of Genovia by Polished for Days 😍</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x39e00120jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1asgufu</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Inspired by my dog's favorite treats</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asgufu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1asgmez</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Good place to buy multiple brands?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1asgmez/good_place_to_buy_multiple_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1asgjjw</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Wanted to try out some polishes. Ended up with this skittle. Not sure if it works but at least I had fun  😊</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzgrajvzvzic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1asg55c</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>One polish shy of a purple skittle</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asg55c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1asfs36</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>LynBDesigns - Puppy Kisses</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asfs36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1asfqqc</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>ILNP Sandy Baby &amp; Cirque Colors Georgette</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asfqqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1aseqtj</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat - Haunted Forest found!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xetk0gwizic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1aselod</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Subtle... let's call it subtle. 👀</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aselod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ase6zz</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>🖼Monet Water Lillies🖼</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ase6zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1asdvxv</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Lucky 13 Lacquers - Wibbly Wobbly Timey Wimey</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asdvxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1asd2mw</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>LynB skittle</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci8a3xd17zic1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1ascso6</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>A Midsummer’s Dream in the snow</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ascso6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1asbwsg</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>A Rose in Death’s Valley</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asbwsg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1asbtv1</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>What do I ask for to get this?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asbtv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1asbpve</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Attempted flowers for the first time and it didn't go as planned 🙃</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kubbo7v8xyic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1asbfo0</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Shimmery Polishes &gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asbfo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1asb4vq</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Starrily Venus</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asb4vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1asatwe</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Cirque brings back $25 grab bags, but the language they use about receiving duplicates just…bothers me…</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0vpr72kqyic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1as9z4x</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Cirque's reflective glitter has me in a chokehold</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as9z4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1as8ti1</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Made myself a tool to do velvet nails, pretty impressed with how they turned out!</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1as8ti1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1asv86l</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Valentine nails &lt;3 nail tech slayed once again</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iaiup3ch93jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1asuk6z</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Scooby Doo Nails 🤠</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6f6empc23jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1asu1ix</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My 2. Nail art ever. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dzwqmt2x2jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1astw67</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>@sweetbobanails is a nail wizard</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1astw67</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1astmoi</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Hand sculpted and hand painted sanrio at the fair custom press on nails by me🎠💕</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1astmoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1asp8yn</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>I forgot to post mine, my moms and my grandmas Valentine’s Day nails! 💌💘 I did them like two weeks ago 🩷</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asp8yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1asobfj</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Strawberry cow</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vefgfzw1i1jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1aslavu</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Pink and dandelion set</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aslavu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1ask50k</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Plankton and Karen my goddess stylist did for me</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ask50k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1asig30</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>pay no mind to my wayward ring position but i do my own nails and i’m quite proud of these ones.</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4c2zsly90jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1ase1sv</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>🔥</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcmt5q41ezic1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1asbsg5</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>I feel like somethings oss</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d4v489sxyic1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Feb 18 08:07:44 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_02_18.xlsx
+++ b/data/2024_02_18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1155"/>
+  <dimension ref="A1:C1312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20068,6 +20068,2675 @@
         </is>
       </c>
     </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1ato9yz</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>I’m a gay guy who’s on the more masculine side. Looking to get my nails done in a way that makes me not want to bite them. What should I tell the workers at the nail salon?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ato9yz/im_a_gay_guy_whos_on_the_more_masculine_side/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1atksmp</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Venom inspired!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atksmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1atfk9o</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Anyone know why this Shellac has discolouration?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atfk9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1atmced</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>My 5 Year Anniversary nails 🖤💗</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbwiq13q2ajc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1atlzth</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Dip powder has ruined my nails — help</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xeztvs4z9jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1atkl1m</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>What do y’all think?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atkl1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1atkke2</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Nothing Stays on my Nails 😤</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1atkke2/nothing_stays_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1atkj81</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8agjdjbk9jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1atke06</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>French tips</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh8x5o0wi9jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1atk3le</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Gel extensions, Hawaiian style</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mwrx4bc3g9jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1atizuu</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>My nails match my shoeer curtain 🌌💅🛸</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atizuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1atipqc</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Very happy with how todays set turned out</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a61l2md39jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1atim2b</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Very pleasantly surprised by these press-ons</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atim2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1atik30</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Vegas Nails!</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvtzg1ny19jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ati8p3</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Manicure chips regardless of where i get them done at.</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ati8p3/manicure_chips_regardless_of_where_i_get_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1ati5fr</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>My new set! Do you like it?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ati5fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ati3w8</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Psychedelic Unicorn 🦄</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j40pbzux8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1athnqo</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>First time trying out French nails ✨</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dag9qcxt8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1ath4i4</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>How bad are they? Give it to me straight :)</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ath4i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1ath2z0</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Chanel Tweed Art</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ath2z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1atgzyg</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Does this make me look shady?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1atgzyg/does_this_make_me_look_shady/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1atg2gw</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Late Valentine Nails 💕 🍒</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jq4h3mxmg8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1atf9x8</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>A classic always 🤍</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d10x1yl8a8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1atf9ij</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Might be my favorite set so far!! nail tech never disappoints me🧡🩵</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atf9ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1atf3w5</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Moo 🐄</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ers5gl6v88jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1atezsx</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>My first at-home gel manicure using an LED lamp!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atezsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1ateyyh</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black and white 60s vibe </t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tb3o16u78jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1atekg4</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Some nail art I did for my mom and dad’s dart tournament!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlca903p48jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ated8t</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>New set for my birthday (press-on)</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv6qycj438jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1atdl30</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>how do i stain gel nails</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1atdl30/how_do_i_stain_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1ataszm</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Are there sample sizing tools for nail extensions?</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ataszm/are_there_sample_sizing_tools_for_nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1at90qv</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>acrylic sculpt</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at90qv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1at8ukt</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>First time doing nails!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eywq95lxw6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1at8fa7</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>My nail is curved?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at8fa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1atdnvx</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>I’m obsessed with chrome</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5cj93rqx7jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1atdlnn</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Broke down and did the two coats Funny Bunny &amp; one coat Bubble Bath. Love them! 😍 I do gel overlay on my natural nails</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atdlnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1atdkf3</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Super rad blue quartz x molten metal nails I did on my client for his birthday 💙⛓️</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atdkf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1atdjvz</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Bears and bows</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgsd1iexw7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1atdhgy</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Do these look odd? First set of acrylics…</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atdhgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1atdb75</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Pink flakes 🌸🤍</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekhyq191v7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1atdack</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Strawbearry nails 🍓🧸💖</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atdack</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1atd96t</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Questions about Gel-X </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1atd96t/questions_about_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1atd523</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes you have to do nails that appeal to your crow brain. ✨️ </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2paz6hdpt7jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1atcxgp</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Is this too much?</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1368muv3s7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1atcq3d</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Idk, I just wanted some silver squiggles.</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hp2fu0ehq7jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1atch2k</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>I’m blue da ba dee…</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atch2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1atceud</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>my favorite set!</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vf02w21o7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1atcb3y</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>What nail shape best suits my hands?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atcb3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1atc87z</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Apres gel removal</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1atc87z/apres_gel_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1atc17o</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried matte black nails. </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb964v01l7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1atbn8g</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Chromies</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atbn8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1atayaw</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Does this pink go well with my skin tone? Let me know!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atayaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1atawrk</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>First attempt at nail design</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mmy8hi6fc7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1atan2g</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>I’m not sure where to post this but is there any fix for this?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atan2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1atal3t</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>literally so obsessed with how this set glitters in the sun light 😩💖</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hexex271a7jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1atac3c</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Artsy Fartsy</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg3p13e787jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1at9yoh</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Its been grey &amp; gloomy in Seattle, WA so we added some pretty color to my nails 💅🏾 😍</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gv1dj4md57jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1at9t81</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>really into blue lately!</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8n130z6847jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1at9m2n</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>The cutest and prettiest nails in my eyes! 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at9m2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1at9aed</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>As much as I am a nail art junkie, this base color is just perfection</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g50zx4b907jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1at8xwy</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>BD Nails for my sister! Do you like them?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/th6p5pwmx6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1at8wdc</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Oil spill chrome!</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h9thx60bx6jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1at8msu</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>New set. Who dis</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s865hdlav6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1at8az4</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>How to decide on nail shape?</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at8az4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1at80c3</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>I’m still wearing red for Heart Disease Awareness Month.</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhnwb07iq6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1at7nps</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>What to do with a crack this far down?</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at7nps</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1at740x</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>A moonstone moment</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at740x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1at72m8</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>First time wearing full hands to work</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbw7mm78j6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1at6srv</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>I call them my goth unicorn nails</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrrka8w8h6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1at6npy</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71ux7m08g6jc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1at5nsk</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Best Hassle-Free Ways to Practice</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1at5nsk/best_hasslefree_ways_to_practice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1at61c1</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Soft Pink Sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i77y55nkb6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1at5svo</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Do you like this colour?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at5svo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1at5gar</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Birthday Nails!</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at5gar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1at5bl6</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>My husband says they remind him of caramel apples 🤎🍏</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh2tvb6w56jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1at57d8</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>New color!</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gyguhg9z46jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1at53ee</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got smokey nails! </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qngqufi346jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1at4qzt</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2nd time doing my nails </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yn7m2c2c16jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1at4ocg</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Maybelline Fast Gel / Sheer Fantasy. It's got a shimmer going on that tbh I'm here for. Was looking for something springy as the days are getting longer.</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzmonaym06jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1at4n1s</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Neutral Chrome✨</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at4n1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1at3oz3</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">first time getting professional gel polish! any tips or advice? </t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcl2l1rns5jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1at42jj</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>My favorite glitter</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at42jj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1at3yp7</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Sculpted French Nails</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8852u7tvu5jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1asuyjm</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Whats happening? I must be sick. 🧟‍♀️ 🧟‍♀️ 🧟‍♀️</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asuyjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1at2ijl</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Last month I posted my "depression recovering" nails here and I got so many positive comments. Thank you everybody 💕❤️💅 it really meant a lot. I hope you like my new set as well</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at2ijl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1at28yw</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>I like it! Do you?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66gxkgw6g5jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1at1mgg</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>How to get your nails strong and pretty?</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1at1mgg/how_to_get_your_nails_strong_and_pretty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1at1adw</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Testing the red nail theory</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at1adw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1at01dg</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Another set 😫❤️</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yda06zzau4jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1asztg3</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>My nail design.</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asztg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1aszh65</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Pretty in pink</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgvp2s6on4jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1asz8nq</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>What type of nail polish is this called?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/li9p28ozk4jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1asyf2g</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>In love with subtle glitter!</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjafrftcb4jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1atoaky</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>My first press-on 🩵</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31dk07c4oajc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1atmxld</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>I'm so glad I got this polish</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atmxld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1atmtb2</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Dupe for Chanel Atmosphere or Dior Perle?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1atmtb2/dupe_for_chanel_atmosphere_or_dior_perle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1atgjht</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>why has no one used this l'oréal gel ultime top coat?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ubo0da7hk8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1atggo6</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>why has no one used this nail polish..please help!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7kctcotj8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1atexb3</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>How do I prevent my nails from looking scuffed?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1atexb3/how_do_i_prevent_my_nails_from_looking_scuffed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1atduox</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Mani Mad Science Update: Magnet Maximization, Two Month Check In</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fm3srd7z7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1atmg40</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>An issue with Orly</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atmg40</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1atlp03</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>ILNP Amber</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfnvemxzv9jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1atkdqh</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Orly - Scenic Route</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atkdqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1atk9ld</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Sugar Plum vs Mooncat Velvet Rose Help! </t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1atk9ld/ilnp_sugar_plum_vs_mooncat_velvet_rose_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1atj1r4</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>My nails match my shower curtain! 🛸💅🌌</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atj1r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1atiq31</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>M&amp;N Indie Polish “Wolfsbane”: Gorgeous but inaccurate to swatches</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atiq31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1athasw</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Home mixed jelly polish</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tc5mui0sq8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1atg3xz</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Fancy Gloss Thermal &amp; Toppers</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atg3xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1atflvf</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Nightshade is the best magnetic I've ever used</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atflvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1atfg0j</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Cock a doodle dooooooom</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atfg0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1atf5lv</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>ILNP “Undenied” - Swipe for the Shifty Shiffff</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atf5lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1atew2l</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>So shifty 💜💙</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atew2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1atel5s</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Boring + 10 mgs of Adderall</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atel5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1ateah5</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>You ever just go way overboard for one manicure?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ateah5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1ate4ub</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>My Friends nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er9e818c18jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1ate2ns</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Angel Wings by Polished for Days</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ate2ns</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1ate1lj</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>CHANEL 637 Malice</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ate1lj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1at94zr</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Boolba - Phoenix (received as PR)</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at94zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1atdjht</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Can I remove regular lacquer without ruining my gel tips?</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1atdjht/can_i_remove_regular_lacquer_without_ruining_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1atcjou</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about wraps! </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1atcjou/question_about_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1atcj3q</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>🥀 Mooncat’s Access Denied🥀 This color✨Everything✨💚🖤</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atcj3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1atbx7d</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Prince of envy</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5po79xt5k7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1atbovt</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Wanted to do something simple for Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0sqye5ai7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1atba97</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Update: I went to Orly's Color Labs and...</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atba97</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ataljh</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Dashing diva lamp for other gel polish?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ataljh/dashing_diva_lamp_for_other_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ataizb</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opalite inspired polish? </t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkh6mxjl97jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1at9bcx</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Eggs!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at9bcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1at9871</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Spent way to long doing this 🧲</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at9871</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1at8x9l</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Back to shorties! And found my favorite one coat polish</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at8x9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1at86qp</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>how long should I wait to apply nail oil after I paint my nails?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1at86qp/how_long_should_i_wait_to_apply_nail_oil_after_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1at7dk0</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Earth Tone Rainbow Skittle</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at7dk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1at7b71</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Saucy Soka</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6lrmoc4l6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1at6f1j</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Petals for a Narcissist glow ✨</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vs1qwouge6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1at5zdc</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>First post</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3a75ew4b6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1at5tkx</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Pink jelly stained my nails 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at5tkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1at5317</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>I’m a beginner nail tech wanting to specialize in gel/freehand nail art!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5pb0iq046jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1at50td</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails | Atropa Belladonna Thermal</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0vm7nxc36jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1at4w6f</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Latte Cloud w/ long nails</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at4w6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1at4kcm</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Tried Death Valley nail polish Shade "Abalone"</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pb8x2hmez5jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1at3wvg</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Asking question for my daughter, about KBShimmer polishes. </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1at3wvg/asking_question_for_my_daughter_about_kbshimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1at3nno</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>My friend is marrying a farmer so I dressed as a cowgirl for her hens night</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u4il5ecs5jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1at3g0n</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is the longest &amp; best my nails have ever looked! </t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmrhj0tjq5jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1at1bxi</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Weekend Nails! 🩶</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfrct8bs75jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1asxi01</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>RIP. (how this ended up going through the washing machine, I'll never know [spoiler: it was the husband])</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txdj3v3yz3jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1asxhwb</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Club Mykonos</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/Eeqv267</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1atov3e</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails </t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usezt6asuajc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1atko9b</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Black &amp; Green combo!</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atko9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1atj2yt</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Feeling The Blues</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atj2yt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1atgqz5</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>yes or no ?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wcb7sj7m8jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1atcire</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Lisa Frank inspired nails!</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atcire</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1atc6nb</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Valentine gift to myself 🎀</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1atc6nb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1atb8ul</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>My cruise set 🤭🤭🤭</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8035tyqze7jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1at9a4b</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>I love my 7am nail appointment. My amazing NT Irina @ lashnnailroom is always ready to start her day and does such a great job!</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at9a4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1at8vou</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Oil spill chrome! I'm in love</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ppix84i5x6jc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1at8qvw</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Reclaimed by Nature 🌿🌷🦟🐊</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1at8qvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1at5wwv</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>JJK (Sukuna) nails I’m super happy with.</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an76ok9ma6jc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1asztpm</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>My nail art work.</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1asztpm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>